<commit_message>
[FEAT] New Vacations Report Template
</commit_message>
<xml_diff>
--- a/config_files/Horarios/Medibiofarma/Alba Velle.xlsx
+++ b/config_files/Horarios/Medibiofarma/Alba Velle.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="470">
   <si>
     <t>Calendario 2022</t>
   </si>
@@ -323,7 +323,8 @@
     <t>Medibiofarma</t>
   </si>
   <si>
-    <t>B66918053</t>
+    <t xml:space="preserve">B66918053
+</t>
   </si>
   <si>
     <t>31/1124914-33</t>
@@ -9416,21 +9417,20 @@
       </c>
     </row>
     <row r="46" ht="15.6" customHeight="true">
-      <c r="Z46" s="104" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="AA46" s="109" t="n">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="AB46" s="109" t="n">
-        <v>0.7083333333333334</v>
-      </c>
-      <c r="AC46" s="106" t="n">
-        <v>8.0</v>
-      </c>
+      <c r="Z46" s="104"/>
+      <c r="AA46" s="109"/>
+      <c r="AB46" s="109"/>
+      <c r="AC46" s="106"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="G1:M1"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="T13:V13"/>
     <mergeCell ref="AA40:AC40"/>
     <mergeCell ref="AA33:AC33"/>
     <mergeCell ref="AA34:AC34"/>
@@ -9440,13 +9440,6 @@
     <mergeCell ref="D32:F32"/>
     <mergeCell ref="L32:N32"/>
     <mergeCell ref="T32:V32"/>
-    <mergeCell ref="G1:M1"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="T13:V13"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Corrected Mid Day Vacations
</commit_message>
<xml_diff>
--- a/config_files/Horarios/Medibiofarma/Alba Velle.xlsx
+++ b/config_files/Horarios/Medibiofarma/Alba Velle.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="118">
   <si>
     <t>Calendario 2022</t>
   </si>
@@ -379,17 +379,20 @@
   <si>
     <t>Diciembre</t>
   </si>
+  <si>
+    <t>0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="ddd"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="d"/>
     <numFmt numFmtId="180" formatCode="mmmm\ yyyy"/>
     <numFmt numFmtId="181" formatCode="[$-40A]d\ mmm;@"/>
@@ -1965,7 +1968,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2282,6 +2285,15 @@
     </xf>
     <xf numFmtId="177" fontId="16" fillId="10" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -3126,16 +3138,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89090909090909" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="2.78181818181818" customWidth="1" collapsed="1"/>
-    <col min="2" max="8" width="6.78181818181818" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="2.78181818181818" customWidth="1" collapsed="1"/>
-    <col min="10" max="16" width="6.78181818181818" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="2.78181818181818" customWidth="1" collapsed="1"/>
-    <col min="18" max="24" width="6.78181818181818" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="10" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.78181818181818" customWidth="1" collapsed="1"/>
-    <col min="27" max="29" width="25" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="10" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="2.78181818181818" collapsed="true"/>
+    <col min="2" max="8" customWidth="true" width="6.78181818181818" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="2.78181818181818" collapsed="true"/>
+    <col min="10" max="16" customWidth="true" width="6.78181818181818" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="2.78181818181818" collapsed="true"/>
+    <col min="18" max="24" customWidth="true" width="6.78181818181818" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="5.78181818181818" collapsed="true"/>
+    <col min="27" max="29" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.8" customHeight="1" spans="2:24">
@@ -5142,18 +5154,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89090909090909" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.8909090909091" customWidth="1"/>
-    <col min="2" max="2" width="18.6636363636364" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="3.10909090909091" customWidth="1"/>
-    <col min="5" max="5" width="18.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="3.10909090909091" customWidth="1"/>
-    <col min="7" max="7" width="14.6636363636364" customWidth="1"/>
-    <col min="8" max="8" width="4.66363636363636" customWidth="1"/>
-    <col min="9" max="9" width="10.8909090909091" customWidth="1"/>
-    <col min="10" max="10" width="5.33636363636364" customWidth="1"/>
-    <col min="11" max="11" width="13.3363636363636" customWidth="1"/>
-    <col min="12" max="17" width="10.8909090909091" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.66363636363636" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33636363636364" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.3363636363636" collapsed="true"/>
+    <col min="12" max="17" customWidth="true" width="10.8909090909091" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="1" spans="10:11">
@@ -5726,18 +5738,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89090909090909" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.8909090909091" customWidth="1"/>
-    <col min="2" max="2" width="18.6636363636364" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="3.10909090909091" customWidth="1"/>
-    <col min="5" max="5" width="18.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="3.10909090909091" customWidth="1"/>
-    <col min="7" max="7" width="14.6636363636364" customWidth="1"/>
-    <col min="8" max="8" width="4.66363636363636" customWidth="1"/>
-    <col min="9" max="9" width="10.8909090909091" customWidth="1"/>
-    <col min="10" max="10" width="5.33636363636364" customWidth="1"/>
-    <col min="11" max="11" width="13.3363636363636" customWidth="1"/>
-    <col min="12" max="17" width="10.8909090909091" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.66363636363636" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33636363636364" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.3363636363636" collapsed="true"/>
+    <col min="12" max="17" customWidth="true" width="10.8909090909091" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="1" spans="10:11">
@@ -6318,18 +6330,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89090909090909" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.8909090909091" customWidth="1"/>
-    <col min="2" max="2" width="18.6636363636364" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="3.10909090909091" customWidth="1"/>
-    <col min="5" max="5" width="18.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="3.10909090909091" customWidth="1"/>
-    <col min="7" max="7" width="14.6636363636364" customWidth="1"/>
-    <col min="8" max="8" width="4.66363636363636" customWidth="1"/>
-    <col min="9" max="9" width="10.8909090909091" customWidth="1"/>
-    <col min="10" max="10" width="5.33636363636364" customWidth="1"/>
-    <col min="11" max="11" width="13.3363636363636" customWidth="1"/>
-    <col min="12" max="17" width="10.8909090909091" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.66363636363636" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33636363636364" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.3363636363636" collapsed="true"/>
+    <col min="12" max="17" customWidth="true" width="10.8909090909091" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="1" spans="10:11">
@@ -6900,18 +6912,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89090909090909" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.8909090909091" customWidth="1"/>
-    <col min="2" max="2" width="18.6636363636364" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="3.10909090909091" customWidth="1"/>
-    <col min="5" max="5" width="18.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="3.10909090909091" customWidth="1"/>
-    <col min="7" max="7" width="14.6636363636364" customWidth="1"/>
-    <col min="8" max="8" width="4.66363636363636" customWidth="1"/>
-    <col min="9" max="9" width="10.8909090909091" customWidth="1"/>
-    <col min="10" max="10" width="5.33636363636364" customWidth="1"/>
-    <col min="11" max="11" width="13.3363636363636" customWidth="1"/>
-    <col min="12" max="17" width="10.8909090909091" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.66363636363636" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33636363636364" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.3363636363636" collapsed="true"/>
+    <col min="12" max="17" customWidth="true" width="10.8909090909091" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="1" spans="10:11">
@@ -7491,18 +7503,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89090909090909" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.8909090909091" customWidth="1"/>
-    <col min="2" max="2" width="18.6636363636364" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="3.10909090909091" customWidth="1"/>
-    <col min="5" max="5" width="18.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="3.10909090909091" customWidth="1"/>
-    <col min="7" max="7" width="14.6636363636364" customWidth="1"/>
-    <col min="8" max="8" width="4.66363636363636" customWidth="1"/>
-    <col min="9" max="9" width="10.8909090909091" customWidth="1"/>
-    <col min="10" max="10" width="5.33636363636364" customWidth="1"/>
-    <col min="11" max="11" width="13.3363636363636" customWidth="1"/>
-    <col min="12" max="17" width="10.8909090909091" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.66363636363636" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33636363636364" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.3363636363636" collapsed="true"/>
+    <col min="12" max="17" customWidth="true" width="10.8909090909091" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="1" spans="10:14">
@@ -8185,18 +8197,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89090909090909" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.8909090909091" customWidth="1"/>
-    <col min="2" max="2" width="18.6636363636364" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="3.10909090909091" customWidth="1"/>
-    <col min="5" max="5" width="18.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="3.10909090909091" customWidth="1"/>
-    <col min="7" max="7" width="14.6636363636364" customWidth="1"/>
-    <col min="8" max="8" width="4.66363636363636" customWidth="1"/>
-    <col min="9" max="9" width="10.8909090909091" customWidth="1"/>
-    <col min="10" max="10" width="5.33636363636364" customWidth="1"/>
-    <col min="11" max="11" width="13.3363636363636" customWidth="1"/>
-    <col min="12" max="17" width="10.8909090909091" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.66363636363636" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33636363636364" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.3363636363636" collapsed="true"/>
+    <col min="12" max="17" customWidth="true" width="10.8909090909091" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="1" spans="10:14">
@@ -8865,18 +8877,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89090909090909" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.8909090909091" customWidth="1"/>
-    <col min="2" max="2" width="18.6636363636364" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="3.10909090909091" customWidth="1"/>
-    <col min="5" max="5" width="18.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="3.10909090909091" customWidth="1"/>
-    <col min="7" max="7" width="14.6636363636364" customWidth="1"/>
-    <col min="8" max="8" width="4.66363636363636" customWidth="1"/>
-    <col min="9" max="9" width="10.8909090909091" customWidth="1"/>
-    <col min="10" max="10" width="5.33636363636364" customWidth="1"/>
-    <col min="11" max="11" width="13.3363636363636" customWidth="1"/>
-    <col min="12" max="17" width="10.8909090909091" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.66363636363636" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33636363636364" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.3363636363636" collapsed="true"/>
+    <col min="12" max="17" customWidth="true" width="10.8909090909091" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="1" spans="10:14">
@@ -9568,18 +9580,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89090909090909" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.8909090909091" customWidth="1"/>
-    <col min="2" max="2" width="18.6636363636364" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="3.10909090909091" customWidth="1"/>
-    <col min="5" max="5" width="18.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="3.10909090909091" customWidth="1"/>
-    <col min="7" max="7" width="14.6636363636364" customWidth="1"/>
-    <col min="8" max="8" width="4.66363636363636" customWidth="1"/>
-    <col min="9" max="9" width="10.8909090909091" customWidth="1"/>
-    <col min="10" max="10" width="5.33636363636364" customWidth="1"/>
-    <col min="11" max="11" width="13.3363636363636" customWidth="1"/>
-    <col min="12" max="17" width="10.8909090909091" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.66363636363636" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33636363636364" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.3363636363636" collapsed="true"/>
+    <col min="12" max="17" customWidth="true" width="10.8909090909091" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="1" spans="10:14">
@@ -10239,18 +10251,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89090909090909" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.8909090909091" customWidth="1"/>
-    <col min="2" max="2" width="18.6636363636364" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="3.10909090909091" customWidth="1"/>
-    <col min="5" max="5" width="18.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="3.10909090909091" customWidth="1"/>
-    <col min="7" max="7" width="14.6636363636364" customWidth="1"/>
-    <col min="8" max="8" width="4.66363636363636" customWidth="1"/>
-    <col min="9" max="9" width="10.8909090909091" customWidth="1"/>
-    <col min="10" max="10" width="5.33636363636364" customWidth="1"/>
-    <col min="11" max="11" width="13.3363636363636" customWidth="1"/>
-    <col min="12" max="17" width="10.8909090909091" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.66363636363636" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33636363636364" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.3363636363636" collapsed="true"/>
+    <col min="12" max="17" customWidth="true" width="10.8909090909091" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="1" spans="10:14">
@@ -10937,18 +10949,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89090909090909" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.8909090909091" customWidth="1"/>
-    <col min="2" max="2" width="18.6636363636364" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="3.10909090909091" customWidth="1"/>
-    <col min="5" max="5" width="18.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="3.10909090909091" customWidth="1"/>
-    <col min="7" max="7" width="14.6636363636364" customWidth="1"/>
-    <col min="8" max="8" width="4.66363636363636" customWidth="1"/>
-    <col min="9" max="9" width="10.8909090909091" customWidth="1"/>
-    <col min="10" max="10" width="5.33636363636364" customWidth="1"/>
-    <col min="11" max="11" width="13.3363636363636" customWidth="1"/>
-    <col min="12" max="17" width="10.8909090909091" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.66363636363636" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33636363636364" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.3363636363636" collapsed="true"/>
+    <col min="12" max="17" customWidth="true" width="10.8909090909091" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="1" spans="10:11">
@@ -11614,18 +11626,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89090909090909" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.8909090909091" customWidth="1"/>
-    <col min="2" max="2" width="18.6636363636364" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="3.10909090909091" customWidth="1"/>
-    <col min="5" max="5" width="18.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="3.10909090909091" customWidth="1"/>
-    <col min="7" max="7" width="14.6636363636364" customWidth="1"/>
-    <col min="8" max="8" width="4.66363636363636" customWidth="1"/>
-    <col min="9" max="9" width="10.8909090909091" customWidth="1"/>
-    <col min="10" max="10" width="5.33636363636364" customWidth="1"/>
-    <col min="11" max="11" width="13.3363636363636" customWidth="1"/>
-    <col min="12" max="17" width="10.8909090909091" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.66363636363636" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33636363636364" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.3363636363636" collapsed="true"/>
+    <col min="12" max="17" customWidth="true" width="10.8909090909091" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="1" spans="10:11">
@@ -11765,11 +11777,11 @@
       <c r="B16" s="12">
         <v>1</v>
       </c>
-      <c r="C16" s="47">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="E16" s="47">
-        <v>0.708333333333333</v>
+      <c r="C16" s="132" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E16" s="132" t="n">
+        <v>0.7083333333333334</v>
       </c>
       <c r="G16" s="11">
         <f t="shared" ref="G16:G20" si="0">IF((E16-C16)*24&lt;=4,(E16-C16)*24,(E16-C16)*24-1)</f>
@@ -11800,11 +11812,11 @@
       <c r="B19" s="12">
         <v>4</v>
       </c>
-      <c r="C19" s="47">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="E19" s="47">
-        <v>0.708333333333333</v>
+      <c r="C19" s="132" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E19" s="132" t="n">
+        <v>0.7083333333333334</v>
       </c>
       <c r="G19" s="11">
         <f t="shared" si="0"/>
@@ -11815,11 +11827,11 @@
       <c r="B20" s="12">
         <v>5</v>
       </c>
-      <c r="C20" s="47">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="E20" s="47">
-        <v>0.708333333333333</v>
+      <c r="C20" s="132" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E20" s="132" t="n">
+        <v>0.7083333333333334</v>
       </c>
       <c r="G20" s="11">
         <f t="shared" si="0"/>
@@ -11892,11 +11904,11 @@
       <c r="B26" s="12">
         <v>11</v>
       </c>
-      <c r="C26" s="47">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="E26" s="47">
-        <v>0.708333333333333</v>
+      <c r="C26" s="132" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E26" s="132" t="n">
+        <v>0.7083333333333334</v>
       </c>
       <c r="G26" s="11">
         <f t="shared" ref="G26:G30" si="1">IF((E26-C26)*24&lt;=4,(E26-C26)*24,(E26-C26)*24-1)</f>
@@ -11907,11 +11919,11 @@
       <c r="B27" s="12">
         <v>12</v>
       </c>
-      <c r="C27" s="47">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="E27" s="47">
-        <v>0.708333333333333</v>
+      <c r="C27" s="132" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E27" s="132" t="n">
+        <v>0.7083333333333334</v>
       </c>
       <c r="G27" s="11">
         <f t="shared" si="1"/>
@@ -11922,11 +11934,11 @@
       <c r="B28" s="12">
         <v>13</v>
       </c>
-      <c r="C28" s="47">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="E28" s="47">
-        <v>0.708333333333333</v>
+      <c r="C28" s="132" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E28" s="132" t="n">
+        <v>0.7083333333333334</v>
       </c>
       <c r="G28" s="11">
         <f t="shared" si="1"/>
@@ -11937,11 +11949,11 @@
       <c r="B29" s="12">
         <v>14</v>
       </c>
-      <c r="C29" s="47">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="E29" s="47">
-        <v>0.708333333333333</v>
+      <c r="C29" s="132" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E29" s="132" t="n">
+        <v>0.7083333333333334</v>
       </c>
       <c r="G29" s="11">
         <f t="shared" si="1"/>
@@ -11952,11 +11964,11 @@
       <c r="B30" s="12">
         <v>15</v>
       </c>
-      <c r="C30" s="47">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="E30" s="47">
-        <v>0.708333333333333</v>
+      <c r="C30" s="132" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E30" s="132" t="n">
+        <v>0.7083333333333334</v>
       </c>
       <c r="G30" s="11">
         <f t="shared" si="1"/>
@@ -11987,11 +11999,11 @@
       <c r="B33" s="12">
         <v>18</v>
       </c>
-      <c r="C33" s="47">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="E33" s="47">
-        <v>0.708333333333333</v>
+      <c r="C33" s="132" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E33" s="132" t="n">
+        <v>0.7083333333333334</v>
       </c>
       <c r="G33" s="11">
         <f t="shared" ref="G33:G37" si="2">IF((E33-C33)*24&lt;=4,(E33-C33)*24,(E33-C33)*24-1)</f>
@@ -12002,11 +12014,11 @@
       <c r="B34" s="12">
         <v>19</v>
       </c>
-      <c r="C34" s="47">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="E34" s="47">
-        <v>0.708333333333333</v>
+      <c r="C34" s="132" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E34" s="132" t="n">
+        <v>0.7083333333333334</v>
       </c>
       <c r="G34" s="11">
         <f t="shared" si="2"/>
@@ -12017,11 +12029,11 @@
       <c r="B35" s="12">
         <v>20</v>
       </c>
-      <c r="C35" s="47">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="E35" s="47">
-        <v>0.708333333333333</v>
+      <c r="C35" s="132" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E35" s="132" t="n">
+        <v>0.7083333333333334</v>
       </c>
       <c r="G35" s="11">
         <f t="shared" si="2"/>
@@ -12032,8 +12044,12 @@
       <c r="B36" s="12">
         <v>21</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="E36" s="13"/>
+      <c r="C36" s="132" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E36" s="132" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G36" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -12043,8 +12059,12 @@
       <c r="B37" s="12">
         <v>22</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="E37" s="13"/>
+      <c r="C37" s="132" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E37" s="132" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G37" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -12084,8 +12104,12 @@
       <c r="B41" s="12">
         <v>26</v>
       </c>
-      <c r="C41" s="13"/>
-      <c r="E41" s="13"/>
+      <c r="C41" s="132" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E41" s="132" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G41" s="11">
         <f t="shared" ref="G41:G44" si="3">IF((E41-C41)*24&lt;=4,(E41-C41)*24,(E41-C41)*24-1)</f>
         <v>0</v>
@@ -12095,8 +12119,12 @@
       <c r="B42" s="12">
         <v>27</v>
       </c>
-      <c r="C42" s="13"/>
-      <c r="E42" s="13"/>
+      <c r="C42" s="132" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E42" s="132" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G42" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -12106,8 +12134,12 @@
       <c r="B43" s="12">
         <v>28</v>
       </c>
-      <c r="C43" s="13"/>
-      <c r="E43" s="13"/>
+      <c r="C43" s="132" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E43" s="132" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G43" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -12117,8 +12149,12 @@
       <c r="B44" s="12">
         <v>29</v>
       </c>
-      <c r="C44" s="13"/>
-      <c r="E44" s="13"/>
+      <c r="C44" s="132" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E44" s="132" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G44" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -12259,18 +12295,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89090909090909" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.8909090909091" customWidth="1"/>
-    <col min="2" max="2" width="18.6636363636364" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="3.10909090909091" customWidth="1"/>
-    <col min="5" max="5" width="18.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="3.10909090909091" customWidth="1"/>
-    <col min="7" max="7" width="14.6636363636364" customWidth="1"/>
-    <col min="8" max="8" width="4.66363636363636" customWidth="1"/>
-    <col min="9" max="9" width="10.8909090909091" customWidth="1"/>
-    <col min="10" max="10" width="5.33636363636364" customWidth="1"/>
-    <col min="11" max="11" width="13.3363636363636" customWidth="1"/>
-    <col min="12" max="17" width="10.8909090909091" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6636363636364" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.10909090909091" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6636363636364" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.66363636363636" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.8909090909091" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33636363636364" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.3363636363636" collapsed="true"/>
+    <col min="12" max="17" customWidth="true" width="10.8909090909091" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="1" spans="10:11">
@@ -12454,11 +12490,14 @@
       <c r="B20" s="12">
         <v>5</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="G20" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="C20" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="21" ht="14.4" customHeight="1" spans="2:7">
@@ -12485,55 +12524,70 @@
       <c r="B23" s="12">
         <v>8</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="G23" s="11">
-        <f t="shared" ref="G23:G27" si="1">IF((E23-C23)*24&lt;=4,(E23-C23)*24,(E23-C23)*24-1)</f>
-        <v>0</v>
+      <c r="C23" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24" ht="14.4" customHeight="1" spans="2:7">
       <c r="B24" s="12">
         <v>9</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="G24" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C24" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="25" ht="14.4" customHeight="1" spans="2:7">
       <c r="B25" s="12">
         <v>10</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="G25" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C25" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="26" ht="14.4" customHeight="1" spans="2:7">
       <c r="B26" s="12">
         <v>11</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="G26" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C26" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="27" ht="14.4" customHeight="1" spans="2:7">
       <c r="B27" s="12">
         <v>12</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="G27" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C27" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="28" ht="14.4" customHeight="1" spans="2:7">
@@ -12570,44 +12624,56 @@
       <c r="B31" s="12">
         <v>16</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="G31" s="11">
-        <f t="shared" ref="G31:G34" si="2">IF((E31-C31)*24&lt;=4,(E31-C31)*24,(E31-C31)*24-1)</f>
-        <v>0</v>
+      <c r="C31" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="32" ht="14.4" customHeight="1" spans="2:7">
       <c r="B32" s="12">
         <v>17</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="G32" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="C32" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="33" ht="14.4" customHeight="1" spans="2:7">
       <c r="B33" s="12">
         <v>18</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="G33" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="C33" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="34" ht="14.4" customHeight="1" spans="2:7">
       <c r="B34" s="12">
         <v>19</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="G34" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="C34" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="35" ht="14.4" customHeight="1" spans="2:7">
@@ -12634,55 +12700,70 @@
       <c r="B37" s="12">
         <v>22</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="G37" s="11">
-        <f t="shared" ref="G37:G41" si="3">IF((E37-C37)*24&lt;=4,(E37-C37)*24,(E37-C37)*24-1)</f>
-        <v>0</v>
+      <c r="C37" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="38" ht="14.4" customHeight="1" spans="2:7">
       <c r="B38" s="12">
         <v>23</v>
       </c>
-      <c r="C38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="G38" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="C38" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="39" ht="14.4" customHeight="1" spans="2:7">
       <c r="B39" s="12">
         <v>24</v>
       </c>
-      <c r="C39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="G39" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="C39" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="40" ht="14.4" customHeight="1" spans="2:7">
       <c r="B40" s="12">
         <v>25</v>
       </c>
-      <c r="C40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="G40" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="C40" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="41" ht="14.4" customHeight="1" spans="2:7">
       <c r="B41" s="12">
         <v>26</v>
       </c>
-      <c r="C41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="G41" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="C41" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="42" ht="14.4" customHeight="1" spans="2:7">
@@ -12709,11 +12790,14 @@
       <c r="B44" s="12">
         <v>29</v>
       </c>
-      <c r="C44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="G44" s="11">
-        <f t="shared" ref="G44:G46" si="4">IF((E44-C44)*24&lt;=4,(E44-C44)*24,(E44-C44)*24-1)</f>
-        <v>0</v>
+      <c r="C44" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="45" ht="14.4" customHeight="1" spans="2:7">
@@ -12723,7 +12807,7 @@
       <c r="C45" s="13"/>
       <c r="E45" s="13"/>
       <c r="G45" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="4" ref="G45:G46">IF((E45-C45)*24&lt;=4,(E45-C45)*24,(E45-C45)*24-1)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>